<commit_message>
create subfolder for maps
</commit_message>
<xml_diff>
--- a/data_log_sheets/TT24_licor_log_file_blank.xlsx
+++ b/data_log_sheets/TT24_licor_log_file_blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2024_TT_phys/data_log_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1938F5A-9903-BF4F-9407-FD2A37198460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E292752-1679-F446-8D26-3A0D7363893B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7300" yWindow="500" windowWidth="34760" windowHeight="28300" xr2:uid="{532FBF57-0CF7-5B48-90F1-3514858F5BF0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -125,12 +125,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -173,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -185,11 +191,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C069A5-AECE-8943-A3CA-2B5D78A6CA67}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="260" zoomScaleNormal="100" zoomScalePageLayoutView="260" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A18" zoomScale="260" zoomScaleNormal="100" zoomScalePageLayoutView="260" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,15 +581,15 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -596,15 +603,15 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -618,15 +625,15 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -640,15 +647,15 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -662,15 +669,15 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -684,15 +691,15 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -706,15 +713,15 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -728,15 +735,15 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -750,15 +757,15 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -771,54 +778,54 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="6" t="s">
         <v>6</v>
       </c>
@@ -830,7 +837,7 @@
     <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="100"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"-,Bold"DATE: _____________
 PLOT: _____________&amp;C&amp;"-,Bold"MACHINE&amp;"-,Regular"

</xml_diff>